<commit_message>
:techonologist: Reordering models folder for better organization
</commit_message>
<xml_diff>
--- a/python-helpers/all-done.xlsx
+++ b/python-helpers/all-done.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\repos\bin-packing\python-helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CDEB29-4E6C-439F-A6B7-7B3234BE9E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766DF479-2F9D-4151-BDEF-3D965EA98A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>

</xml_diff>

<commit_message>
:technologist: Massive data files upload
</commit_message>
<xml_diff>
--- a/python-helpers/all-done.xlsx
+++ b/python-helpers/all-done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\repos\bin-packing\python-helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766DF479-2F9D-4151-BDEF-3D965EA98A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAF7831-1649-447F-B0A8-0A7F2F25DA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="438">
   <si>
     <t>Job number</t>
   </si>
@@ -1098,13 +1098,265 @@
   </si>
   <si>
     <t>csmlLjtO</t>
+  </si>
+  <si>
+    <t>RqQkUGfl</t>
+  </si>
+  <si>
+    <t>xTrvzYsl</t>
+  </si>
+  <si>
+    <t>KSucRkZw</t>
+  </si>
+  <si>
+    <t>FAPfUMyI</t>
+  </si>
+  <si>
+    <t>yeTdSuMp</t>
+  </si>
+  <si>
+    <t>UZMIryfE</t>
+  </si>
+  <si>
+    <t>ljLTnDMJ</t>
+  </si>
+  <si>
+    <t>bCqsIEXA</t>
+  </si>
+  <si>
+    <t>RIHScsgq</t>
+  </si>
+  <si>
+    <t>pKSnslXb</t>
+  </si>
+  <si>
+    <t>JaOflxAT</t>
+  </si>
+  <si>
+    <t>YAVTBgRW</t>
+  </si>
+  <si>
+    <t>JbWUCBXA</t>
+  </si>
+  <si>
+    <t>gseqFMZv</t>
+  </si>
+  <si>
+    <t>XOGIwqLD</t>
+  </si>
+  <si>
+    <t>twTGeVrP</t>
+  </si>
+  <si>
+    <t>ibXswuHC</t>
+  </si>
+  <si>
+    <t>ohgEyKuv</t>
+  </si>
+  <si>
+    <t>fkzLKIsE</t>
+  </si>
+  <si>
+    <t>tcXqsOSp</t>
+  </si>
+  <si>
+    <t>lRDOberF</t>
+  </si>
+  <si>
+    <t>DycZWgrY</t>
+  </si>
+  <si>
+    <t>oKFTPjCu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> qcAypJNj</t>
+  </si>
+  <si>
+    <t>lfevdzIP</t>
+  </si>
+  <si>
+    <t>eRrvNswd</t>
+  </si>
+  <si>
+    <t>atxbgpPO</t>
+  </si>
+  <si>
+    <t>XSaAVzuO</t>
+  </si>
+  <si>
+    <t>yJuCzXqU</t>
+  </si>
+  <si>
+    <t>FtWkRxAu</t>
+  </si>
+  <si>
+    <t>kqPCdojN</t>
+  </si>
+  <si>
+    <t>IHBjdhbW</t>
+  </si>
+  <si>
+    <t>YVRXjETu</t>
+  </si>
+  <si>
+    <t>HUYGaxVT</t>
+  </si>
+  <si>
+    <t>ZgPyQbqv</t>
+  </si>
+  <si>
+    <t>XVFmeGIY</t>
+  </si>
+  <si>
+    <t>DpGHCsAx</t>
+  </si>
+  <si>
+    <t>oKFsnWuX</t>
+  </si>
+  <si>
+    <t>XdeAuvsn</t>
+  </si>
+  <si>
+    <t>svkWqdwy</t>
+  </si>
+  <si>
+    <t>qeBPtkaJ</t>
+  </si>
+  <si>
+    <t>uSanMiXy</t>
+  </si>
+  <si>
+    <t>MYvDlBWm</t>
+  </si>
+  <si>
+    <t>etVqvEdG</t>
+  </si>
+  <si>
+    <t>KbCAfodE</t>
+  </si>
+  <si>
+    <t>BQeNEZnP</t>
+  </si>
+  <si>
+    <t>pnfOqNeU</t>
+  </si>
+  <si>
+    <t>GpJSxCZj</t>
+  </si>
+  <si>
+    <t>yTjBKCaf</t>
+  </si>
+  <si>
+    <t>oNnKFPZJ</t>
+  </si>
+  <si>
+    <t>IEiJrUYb</t>
+  </si>
+  <si>
+    <t>MiPflrUu</t>
+  </si>
+  <si>
+    <t>LSoFeJrU</t>
+  </si>
+  <si>
+    <t>cyIfirCN</t>
+  </si>
+  <si>
+    <t>HfTalOEp</t>
+  </si>
+  <si>
+    <t>bfzedxQN</t>
+  </si>
+  <si>
+    <t>mTxslGyY</t>
+  </si>
+  <si>
+    <t>XIYBUKjJ</t>
+  </si>
+  <si>
+    <t>GubxNQEM</t>
+  </si>
+  <si>
+    <t>VKCDqPkt</t>
+  </si>
+  <si>
+    <t>wJnbptfx</t>
+  </si>
+  <si>
+    <t>XwtTbHly</t>
+  </si>
+  <si>
+    <t>XyqzTaAp</t>
+  </si>
+  <si>
+    <t>kOxslWob</t>
+  </si>
+  <si>
+    <t>RGoZarcM</t>
+  </si>
+  <si>
+    <t>RpFuYWMN</t>
+  </si>
+  <si>
+    <t>nmGzqJYT</t>
+  </si>
+  <si>
+    <t>bcBqNtiU</t>
+  </si>
+  <si>
+    <t>QfTWZxyv</t>
+  </si>
+  <si>
+    <t>cdksqAim</t>
+  </si>
+  <si>
+    <t>TzlDsSQB</t>
+  </si>
+  <si>
+    <t>McZAXDfa</t>
+  </si>
+  <si>
+    <t>fXzbGUOo</t>
+  </si>
+  <si>
+    <t>CJmRrjDg</t>
+  </si>
+  <si>
+    <t>UjYhzdmf</t>
+  </si>
+  <si>
+    <t>uTdCSrAa</t>
+  </si>
+  <si>
+    <t>egNYfQmI</t>
+  </si>
+  <si>
+    <t>OiaoATry</t>
+  </si>
+  <si>
+    <t>BZFJKGvp</t>
+  </si>
+  <si>
+    <t>HxJBTGPt</t>
+  </si>
+  <si>
+    <t>EwIrjAvG</t>
+  </si>
+  <si>
+    <t>DcyLvMkH</t>
+  </si>
+  <si>
+    <t>lGNAKZpg</t>
+  </si>
+  <si>
+    <t>SdLlIcry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1132,6 +1384,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1153,7 +1412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1165,6 +1424,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1445,15 +1707,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C494"/>
+  <dimension ref="A1:C1071"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A474" workbookViewId="0">
-      <selection activeCell="B495" sqref="B495"/>
+    <sheetView tabSelected="1" topLeftCell="A1052" workbookViewId="0">
+      <selection activeCell="A1066" sqref="A1066:B1071"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5410,6 +5672,4622 @@
         <v>353</v>
       </c>
     </row>
+    <row r="495" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A495" s="2">
+        <v>16489776</v>
+      </c>
+      <c r="B495" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A496" s="2">
+        <v>16489895</v>
+      </c>
+      <c r="B496" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A497">
+        <v>16490420</v>
+      </c>
+      <c r="B497" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A498">
+        <v>16490422</v>
+      </c>
+      <c r="B498" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A499">
+        <v>16490424</v>
+      </c>
+      <c r="B499" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A500">
+        <v>16490471</v>
+      </c>
+      <c r="B500" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A501">
+        <v>16490474</v>
+      </c>
+      <c r="B501" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="502" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A502">
+        <v>16490478</v>
+      </c>
+      <c r="B502" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="503" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A503">
+        <v>16490480</v>
+      </c>
+      <c r="B503" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="504" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A504" s="1">
+        <v>16487823</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="505" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A505" s="2">
+        <v>15972729</v>
+      </c>
+      <c r="B505" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="506" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A506" s="2">
+        <v>15972732</v>
+      </c>
+      <c r="B506" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="507" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A507" s="2">
+        <v>15972739</v>
+      </c>
+      <c r="B507" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="508" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A508" s="2">
+        <v>15972742</v>
+      </c>
+      <c r="B508" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="509" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A509" s="2">
+        <v>15972757</v>
+      </c>
+      <c r="B509" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="510" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A510" s="2">
+        <v>15972774</v>
+      </c>
+      <c r="B510" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="511" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A511" s="2">
+        <v>15972770</v>
+      </c>
+      <c r="B511" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="512" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A512" s="2">
+        <v>15972781</v>
+      </c>
+      <c r="B512" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="513" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A513" s="2">
+        <v>15972787</v>
+      </c>
+      <c r="B513" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="514" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A514" s="2">
+        <v>15972792</v>
+      </c>
+      <c r="B514" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="515" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A515" s="2">
+        <v>15972799</v>
+      </c>
+      <c r="B515" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="516" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A516" s="2">
+        <v>15972801</v>
+      </c>
+      <c r="B516" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="517" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A517" s="2">
+        <v>15972869</v>
+      </c>
+      <c r="B517" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="518" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A518" s="2">
+        <v>15972871</v>
+      </c>
+      <c r="B518" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="519" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A519" s="2">
+        <v>15972873</v>
+      </c>
+      <c r="B519" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="520" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A520" s="2">
+        <v>15972911</v>
+      </c>
+      <c r="B520" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="521" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A521" s="2">
+        <v>15972914</v>
+      </c>
+      <c r="B521" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="522" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A522" s="2">
+        <v>15972916</v>
+      </c>
+      <c r="B522" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="523" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A523" s="2">
+        <v>15972961</v>
+      </c>
+      <c r="B523" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="524" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A524" s="2">
+        <v>15972964</v>
+      </c>
+      <c r="B524" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="525" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A525" s="2">
+        <v>15973107</v>
+      </c>
+      <c r="B525" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="526" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A526" s="2">
+        <v>15973108</v>
+      </c>
+      <c r="B526" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="527" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A527" s="2">
+        <v>15973111</v>
+      </c>
+      <c r="B527" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="528" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A528" s="2">
+        <v>15973114</v>
+      </c>
+      <c r="B528" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="529" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A529" s="2">
+        <v>15973119</v>
+      </c>
+      <c r="B529" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="530" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A530" s="2">
+        <v>15973121</v>
+      </c>
+      <c r="B530" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="531" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A531" s="2">
+        <v>15973123</v>
+      </c>
+      <c r="B531" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A532" s="2">
+        <v>15973128</v>
+      </c>
+      <c r="B532" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="533" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A533" s="2">
+        <v>15973130</v>
+      </c>
+      <c r="B533" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="534" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A534" s="2">
+        <v>15973133</v>
+      </c>
+      <c r="B534" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A535" s="2">
+        <v>15973136</v>
+      </c>
+      <c r="B535" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="536" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A536" s="2">
+        <v>15973138</v>
+      </c>
+      <c r="B536" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="537" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A537" s="2">
+        <v>15973141</v>
+      </c>
+      <c r="B537" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="538" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A538" s="2">
+        <v>15973142</v>
+      </c>
+      <c r="B538" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="539" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A539" s="2">
+        <v>15973145</v>
+      </c>
+      <c r="B539" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="540" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A540" s="2">
+        <v>15973148</v>
+      </c>
+      <c r="B540" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="541" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A541" s="2">
+        <v>15974973</v>
+      </c>
+      <c r="B541" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="542" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A542" s="2">
+        <v>15975008</v>
+      </c>
+      <c r="B542" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="543" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A543" s="2">
+        <v>15975025</v>
+      </c>
+      <c r="B543" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A544" s="2">
+        <v>15975038</v>
+      </c>
+      <c r="B544" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="545" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A545" s="2">
+        <v>15975060</v>
+      </c>
+      <c r="B545" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="546" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A546" s="2">
+        <v>15975072</v>
+      </c>
+      <c r="B546" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="547" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A547" s="2">
+        <v>15975080</v>
+      </c>
+      <c r="B547" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="548" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A548" s="2">
+        <v>15975088</v>
+      </c>
+      <c r="B548" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="549" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A549" s="2">
+        <v>15975101</v>
+      </c>
+      <c r="B549" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="550" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A550" s="2">
+        <v>15975105</v>
+      </c>
+      <c r="B550" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="551" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A551" s="2">
+        <v>15975117</v>
+      </c>
+      <c r="B551" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="552" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A552" s="2">
+        <v>15975123</v>
+      </c>
+      <c r="B552" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="553" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A553" s="2">
+        <v>15975126</v>
+      </c>
+      <c r="B553" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="554" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A554" s="2">
+        <v>15975129</v>
+      </c>
+      <c r="B554" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="555" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A555" s="2">
+        <v>15975133</v>
+      </c>
+      <c r="B555" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="556" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A556" s="2">
+        <v>15975136</v>
+      </c>
+      <c r="B556" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="557" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A557" s="2">
+        <v>15975141</v>
+      </c>
+      <c r="B557" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="558" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A558" s="2">
+        <v>15975202</v>
+      </c>
+      <c r="B558" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="559" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A559" s="2">
+        <v>15975210</v>
+      </c>
+      <c r="B559" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="560" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A560" s="2">
+        <v>15975216</v>
+      </c>
+      <c r="B560" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A561" s="2">
+        <v>15975218</v>
+      </c>
+      <c r="B561" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="562" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A562" s="2">
+        <v>15975221</v>
+      </c>
+      <c r="B562" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="563" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A563" s="2">
+        <v>15975230</v>
+      </c>
+      <c r="B563" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="564" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A564" s="2">
+        <v>15975233</v>
+      </c>
+      <c r="B564" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="565" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A565" s="2">
+        <v>15975245</v>
+      </c>
+      <c r="B565" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="566" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A566" s="2">
+        <v>15975276</v>
+      </c>
+      <c r="B566" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="567" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A567" s="2">
+        <v>15975291</v>
+      </c>
+      <c r="B567" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="568" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A568" s="2">
+        <v>15975653</v>
+      </c>
+      <c r="B568" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="569" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A569" s="2">
+        <v>15975667</v>
+      </c>
+      <c r="B569" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="570" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A570" s="2">
+        <v>15975695</v>
+      </c>
+      <c r="B570" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="571" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A571" s="2">
+        <v>15975700</v>
+      </c>
+      <c r="B571" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="572" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A572" s="2">
+        <v>15975712</v>
+      </c>
+      <c r="B572" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="573" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A573" s="2">
+        <v>15975768</v>
+      </c>
+      <c r="B573" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="574" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A574" s="2">
+        <v>15979389</v>
+      </c>
+      <c r="B574" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="575" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A575" s="2">
+        <v>15979395</v>
+      </c>
+      <c r="B575" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="576" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A576" s="2">
+        <v>15979410</v>
+      </c>
+      <c r="B576" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="577" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A577" s="2">
+        <v>15979413</v>
+      </c>
+      <c r="B577" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="578" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A578" s="2">
+        <v>15979419</v>
+      </c>
+      <c r="B578" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="579" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A579" s="2">
+        <v>15979426</v>
+      </c>
+      <c r="B579" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="580" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A580" s="2">
+        <v>15979437</v>
+      </c>
+      <c r="B580" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="581" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A581" s="2">
+        <v>15979446</v>
+      </c>
+      <c r="B581" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="582" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A582" s="2">
+        <v>15979449</v>
+      </c>
+      <c r="B582" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A583" s="2">
+        <v>15979572</v>
+      </c>
+      <c r="B583" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="584" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A584" s="2">
+        <v>15979575</v>
+      </c>
+      <c r="B584" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="585" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A585" s="2">
+        <v>15979578</v>
+      </c>
+      <c r="B585" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="586" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A586" s="2">
+        <v>15979581</v>
+      </c>
+      <c r="B586" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="587" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A587" s="2">
+        <v>15979584</v>
+      </c>
+      <c r="B587" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="588" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A588" s="2">
+        <v>15979587</v>
+      </c>
+      <c r="B588" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="589" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A589" s="2">
+        <v>15979591</v>
+      </c>
+      <c r="B589" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="590" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A590" s="2">
+        <v>15979830</v>
+      </c>
+      <c r="B590" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="591" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A591" s="2">
+        <v>15979832</v>
+      </c>
+      <c r="B591" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="592" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A592" s="2">
+        <v>15979833</v>
+      </c>
+      <c r="B592" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="593" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A593" s="2">
+        <v>15979835</v>
+      </c>
+      <c r="B593" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="594" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A594" s="2">
+        <v>15979858</v>
+      </c>
+      <c r="B594" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="595" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A595" s="2">
+        <v>15979862</v>
+      </c>
+      <c r="B595" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A596" s="2">
+        <v>15979866</v>
+      </c>
+      <c r="B596" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A597" s="2">
+        <v>15979883</v>
+      </c>
+      <c r="B597" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="598" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A598" s="2">
+        <v>15979885</v>
+      </c>
+      <c r="B598" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="599" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A599" s="2">
+        <v>15979886</v>
+      </c>
+      <c r="B599" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="600" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A600" s="2">
+        <v>15979890</v>
+      </c>
+      <c r="B600" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="601" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A601" s="2">
+        <v>15979896</v>
+      </c>
+      <c r="B601" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A602" s="2">
+        <v>15979901</v>
+      </c>
+      <c r="B602" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A603" s="2">
+        <v>15979903</v>
+      </c>
+      <c r="B603" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A604" s="2">
+        <v>15979907</v>
+      </c>
+      <c r="B604" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="605" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A605" s="2">
+        <v>15979912</v>
+      </c>
+      <c r="B605" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A606" s="2">
+        <v>15979923</v>
+      </c>
+      <c r="B606" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="607" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A607" s="2">
+        <v>15979928</v>
+      </c>
+      <c r="B607" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="608" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A608" s="2">
+        <v>15979931</v>
+      </c>
+      <c r="B608" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="609" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A609" s="2">
+        <v>15980025</v>
+      </c>
+      <c r="B609" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="610" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A610" s="2">
+        <v>15980034</v>
+      </c>
+      <c r="B610" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A611" s="2">
+        <v>15980042</v>
+      </c>
+      <c r="B611" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="612" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A612" s="2">
+        <v>15980050</v>
+      </c>
+      <c r="B612" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="613" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A613" s="2">
+        <v>15980055</v>
+      </c>
+      <c r="B613" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A614" s="2">
+        <v>15980061</v>
+      </c>
+      <c r="B614" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="615" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A615" s="2">
+        <v>15980065</v>
+      </c>
+      <c r="B615" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="616" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A616" s="2">
+        <v>15980081</v>
+      </c>
+      <c r="B616" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="617" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A617" s="2">
+        <v>15980313</v>
+      </c>
+      <c r="B617" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="618" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A618" s="2">
+        <v>15980319</v>
+      </c>
+      <c r="B618" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="619" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A619" s="2">
+        <v>15980324</v>
+      </c>
+      <c r="B619" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="620" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A620" s="2">
+        <v>15980333</v>
+      </c>
+      <c r="B620" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="621" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A621" s="2">
+        <v>15980337</v>
+      </c>
+      <c r="B621" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="622" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A622" s="2">
+        <v>15980346</v>
+      </c>
+      <c r="B622" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="623" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A623" s="2">
+        <v>15980761</v>
+      </c>
+      <c r="B623" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="624" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A624" s="2">
+        <v>15980762</v>
+      </c>
+      <c r="B624" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="625" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A625" s="2">
+        <v>15980783</v>
+      </c>
+      <c r="B625" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="626" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A626" s="2">
+        <v>15980784</v>
+      </c>
+      <c r="B626" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="627" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A627" s="2">
+        <v>15980785</v>
+      </c>
+      <c r="B627" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="628" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A628" s="2">
+        <v>15980786</v>
+      </c>
+      <c r="B628" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="629" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A629" s="2">
+        <v>15980788</v>
+      </c>
+      <c r="B629" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="630" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A630" s="2">
+        <v>15980789</v>
+      </c>
+      <c r="B630" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="631" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A631" s="2">
+        <v>15980790</v>
+      </c>
+      <c r="B631" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="632" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A632" s="2">
+        <v>15980791</v>
+      </c>
+      <c r="B632" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="633" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A633" s="2">
+        <v>15980793</v>
+      </c>
+      <c r="B633" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="634" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A634" s="2">
+        <v>15980832</v>
+      </c>
+      <c r="B634" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="635" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A635" s="2">
+        <v>15980835</v>
+      </c>
+      <c r="B635" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="636" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A636" s="2">
+        <v>15980836</v>
+      </c>
+      <c r="B636" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="637" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A637" s="2">
+        <v>15980838</v>
+      </c>
+      <c r="B637" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="638" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A638" s="2">
+        <v>15980841</v>
+      </c>
+      <c r="B638" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="639" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A639" s="2">
+        <v>15980843</v>
+      </c>
+      <c r="B639" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="640" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A640" s="2">
+        <v>15980844</v>
+      </c>
+      <c r="B640" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="641" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A641" s="2">
+        <v>15980847</v>
+      </c>
+      <c r="B641" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="642" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A642" s="2">
+        <v>15980848</v>
+      </c>
+      <c r="B642" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="643" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A643" s="2">
+        <v>15980850</v>
+      </c>
+      <c r="B643" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="644" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A644" s="2">
+        <v>15980851</v>
+      </c>
+      <c r="B644" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="645" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A645" s="2">
+        <v>15980854</v>
+      </c>
+      <c r="B645" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="646" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A646" s="2">
+        <v>15980856</v>
+      </c>
+      <c r="B646" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="647" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A647" s="2">
+        <v>15980860</v>
+      </c>
+      <c r="B647" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="648" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A648" s="2">
+        <v>15980863</v>
+      </c>
+      <c r="B648" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="649" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A649" s="2">
+        <v>15980865</v>
+      </c>
+      <c r="B649" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="650" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A650" s="2">
+        <v>15980867</v>
+      </c>
+      <c r="B650" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="651" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A651" s="2">
+        <v>15980892</v>
+      </c>
+      <c r="B651" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="652" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A652" s="2">
+        <v>15981517</v>
+      </c>
+      <c r="B652" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="653" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A653" s="2">
+        <v>15981536</v>
+      </c>
+      <c r="B653" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="654" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A654" s="2">
+        <v>15981599</v>
+      </c>
+      <c r="B654" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A655" s="2">
+        <v>15981622</v>
+      </c>
+      <c r="B655" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="656" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A656" s="2">
+        <v>15981626</v>
+      </c>
+      <c r="B656" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="657" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A657" s="2">
+        <v>15981871</v>
+      </c>
+      <c r="B657" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="658" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A658" s="2">
+        <v>15981873</v>
+      </c>
+      <c r="B658" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="659" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A659" s="2">
+        <v>15981880</v>
+      </c>
+      <c r="B659" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="660" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A660" s="2">
+        <v>15981881</v>
+      </c>
+      <c r="B660" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="661" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A661" s="2">
+        <v>15981887</v>
+      </c>
+      <c r="B661" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="662" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A662" s="2">
+        <v>15981892</v>
+      </c>
+      <c r="B662" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="663" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A663" s="2">
+        <v>15981894</v>
+      </c>
+      <c r="B663" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="664" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A664" s="2">
+        <v>15981897</v>
+      </c>
+      <c r="B664" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="665" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A665" s="2">
+        <v>15981898</v>
+      </c>
+      <c r="B665" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="666" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A666" s="2">
+        <v>15981948</v>
+      </c>
+      <c r="B666" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="667" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A667" s="2">
+        <v>15981949</v>
+      </c>
+      <c r="B667" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="668" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A668" s="2">
+        <v>15981952</v>
+      </c>
+      <c r="B668" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="669" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A669" s="2">
+        <v>15982119</v>
+      </c>
+      <c r="B669" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="670" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A670" s="2">
+        <v>15982129</v>
+      </c>
+      <c r="B670" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="671" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A671" s="2">
+        <v>15982132</v>
+      </c>
+      <c r="B671" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="672" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A672" s="2">
+        <v>15982135</v>
+      </c>
+      <c r="B672" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="673" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A673" s="2">
+        <v>15982138</v>
+      </c>
+      <c r="B673" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="674" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A674" s="2">
+        <v>15982141</v>
+      </c>
+      <c r="B674" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="675" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A675" s="2">
+        <v>15982153</v>
+      </c>
+      <c r="B675" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="676" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A676" s="2">
+        <v>15982379</v>
+      </c>
+      <c r="B676" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="677" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A677" s="2">
+        <v>15982382</v>
+      </c>
+      <c r="B677" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="678" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A678" s="2">
+        <v>15982408</v>
+      </c>
+      <c r="B678" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="679" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A679" s="2">
+        <v>15982414</v>
+      </c>
+      <c r="B679" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="680" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A680" s="2">
+        <v>15982903</v>
+      </c>
+      <c r="B680" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="681" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A681" s="2">
+        <v>15982905</v>
+      </c>
+      <c r="B681" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A682" s="2">
+        <v>15982906</v>
+      </c>
+      <c r="B682" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A683" s="2">
+        <v>15982908</v>
+      </c>
+      <c r="B683" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A684" s="2">
+        <v>15982910</v>
+      </c>
+      <c r="B684" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A685" s="2">
+        <v>15982912</v>
+      </c>
+      <c r="B685" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A686" s="2">
+        <v>15982918</v>
+      </c>
+      <c r="B686" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A687" s="2">
+        <v>15982921</v>
+      </c>
+      <c r="B687" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A688" s="2">
+        <v>15982924</v>
+      </c>
+      <c r="B688" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A689" s="2">
+        <v>15982931</v>
+      </c>
+      <c r="B689" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A690" s="2">
+        <v>15982937</v>
+      </c>
+      <c r="B690" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A691" s="2">
+        <v>15982938</v>
+      </c>
+      <c r="B691" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A692" s="2">
+        <v>15982941</v>
+      </c>
+      <c r="B692" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A693" s="2">
+        <v>15982942</v>
+      </c>
+      <c r="B693" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A694" s="2">
+        <v>15984046</v>
+      </c>
+      <c r="B694" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A695" s="2">
+        <v>15984048</v>
+      </c>
+      <c r="B695" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A696" s="2">
+        <v>15984052</v>
+      </c>
+      <c r="B696" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A697" s="2">
+        <v>15984085</v>
+      </c>
+      <c r="B697" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="698" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A698" s="2">
+        <v>15984086</v>
+      </c>
+      <c r="B698" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A699" s="2">
+        <v>15984087</v>
+      </c>
+      <c r="B699" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A700" s="2">
+        <v>15984088</v>
+      </c>
+      <c r="B700" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A701" s="2">
+        <v>15984089</v>
+      </c>
+      <c r="B701" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="702" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A702" s="2">
+        <v>15984090</v>
+      </c>
+      <c r="B702" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="703" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A703" s="2">
+        <v>15984091</v>
+      </c>
+      <c r="B703" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="704" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A704" s="2">
+        <v>15984093</v>
+      </c>
+      <c r="B704" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A705" s="2">
+        <v>15984095</v>
+      </c>
+      <c r="B705" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A706" s="2">
+        <v>15984105</v>
+      </c>
+      <c r="B706" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A707" s="2">
+        <v>15984106</v>
+      </c>
+      <c r="B707" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A708" s="2">
+        <v>15984109</v>
+      </c>
+      <c r="B708" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A709" s="2">
+        <v>15984172</v>
+      </c>
+      <c r="B709" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="710" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A710" s="2">
+        <v>15984174</v>
+      </c>
+      <c r="B710" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A711" s="2">
+        <v>15984175</v>
+      </c>
+      <c r="B711" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A712" s="2">
+        <v>15984176</v>
+      </c>
+      <c r="B712" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A713" s="2">
+        <v>15984189</v>
+      </c>
+      <c r="B713" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="714" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A714" s="2">
+        <v>15984190</v>
+      </c>
+      <c r="B714" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="715" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A715" s="2">
+        <v>15984191</v>
+      </c>
+      <c r="B715" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="716" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A716" s="2">
+        <v>15984213</v>
+      </c>
+      <c r="B716" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="717" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A717" s="2">
+        <v>15984216</v>
+      </c>
+      <c r="B717" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="718" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A718" s="2">
+        <v>15984218</v>
+      </c>
+      <c r="B718" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="719" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A719" s="2">
+        <v>15984231</v>
+      </c>
+      <c r="B719" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="720" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A720" s="2">
+        <v>15984233</v>
+      </c>
+      <c r="B720" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A721" s="2">
+        <v>15984256</v>
+      </c>
+      <c r="B721" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A722" s="2">
+        <v>15984264</v>
+      </c>
+      <c r="B722" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="723" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A723" s="2">
+        <v>15984265</v>
+      </c>
+      <c r="B723" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="724" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A724" s="2">
+        <v>15984287</v>
+      </c>
+      <c r="B724" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="725" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A725" s="2">
+        <v>15984290</v>
+      </c>
+      <c r="B725" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="726" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A726" s="2">
+        <v>15984314</v>
+      </c>
+      <c r="B726" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="727" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A727" s="2">
+        <v>15984316</v>
+      </c>
+      <c r="B727" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A728" s="2">
+        <v>15984321</v>
+      </c>
+      <c r="B728" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A729" s="2">
+        <v>15984324</v>
+      </c>
+      <c r="B729" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="730" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A730" s="2">
+        <v>15984328</v>
+      </c>
+      <c r="B730" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A731" s="2">
+        <v>15984330</v>
+      </c>
+      <c r="B731" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A732" s="2">
+        <v>15988035</v>
+      </c>
+      <c r="B732" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A733" s="2">
+        <v>15988036</v>
+      </c>
+      <c r="B733" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="734" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A734" s="2">
+        <v>15988039</v>
+      </c>
+      <c r="B734" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A735" s="2">
+        <v>15988041</v>
+      </c>
+      <c r="B735" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="736" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A736" s="2">
+        <v>15988042</v>
+      </c>
+      <c r="B736" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="737" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A737" s="2">
+        <v>15988044</v>
+      </c>
+      <c r="B737" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="738" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A738" s="2">
+        <v>15988045</v>
+      </c>
+      <c r="B738" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="739" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A739" s="2">
+        <v>15988049</v>
+      </c>
+      <c r="B739" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="740" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A740" s="2">
+        <v>15988053</v>
+      </c>
+      <c r="B740" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="741" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A741" s="2">
+        <v>15988054</v>
+      </c>
+      <c r="B741" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="742" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A742" s="2">
+        <v>15988055</v>
+      </c>
+      <c r="B742" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A743" s="2">
+        <v>15988056</v>
+      </c>
+      <c r="B743" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="744" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A744" s="2">
+        <v>15988058</v>
+      </c>
+      <c r="B744" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="745" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A745" s="2">
+        <v>15988069</v>
+      </c>
+      <c r="B745" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="746" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A746" s="2">
+        <v>15988070</v>
+      </c>
+      <c r="B746" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="747" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A747" s="2">
+        <v>15991291</v>
+      </c>
+      <c r="B747" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A748" s="2">
+        <v>15991309</v>
+      </c>
+      <c r="B748" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A749" s="2">
+        <v>15992262</v>
+      </c>
+      <c r="B749" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="750" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A750" s="2">
+        <v>15992273</v>
+      </c>
+      <c r="B750" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="751" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A751" s="2">
+        <v>15992318</v>
+      </c>
+      <c r="B751" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A752" s="2">
+        <v>15992325</v>
+      </c>
+      <c r="B752" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A753" s="2">
+        <v>15992338</v>
+      </c>
+      <c r="B753" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A754" s="2">
+        <v>15992341</v>
+      </c>
+      <c r="B754" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A755" s="2">
+        <v>15992358</v>
+      </c>
+      <c r="B755" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="756" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A756" s="2">
+        <v>15992364</v>
+      </c>
+      <c r="B756" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="757" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A757" s="2">
+        <v>15992365</v>
+      </c>
+      <c r="B757" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="758" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A758" s="2">
+        <v>15992367</v>
+      </c>
+      <c r="B758" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="759" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A759" s="2">
+        <v>15992405</v>
+      </c>
+      <c r="B759" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="760" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A760" s="2">
+        <v>15992415</v>
+      </c>
+      <c r="B760" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="761" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A761" s="2">
+        <v>15992418</v>
+      </c>
+      <c r="B761" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="762" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A762" s="2">
+        <v>15992419</v>
+      </c>
+      <c r="B762" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="763" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A763" s="2">
+        <v>15994989</v>
+      </c>
+      <c r="B763" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="764" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A764" s="2">
+        <v>15994999</v>
+      </c>
+      <c r="B764" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="765" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A765" s="2">
+        <v>15995009</v>
+      </c>
+      <c r="B765" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="766" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A766" s="2">
+        <v>15995033</v>
+      </c>
+      <c r="B766" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="767" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A767" s="2">
+        <v>15995038</v>
+      </c>
+      <c r="B767" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="768" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A768" s="2">
+        <v>15995106</v>
+      </c>
+      <c r="B768" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="769" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A769" s="2">
+        <v>15995115</v>
+      </c>
+      <c r="B769" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="770" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A770" s="2">
+        <v>15995118</v>
+      </c>
+      <c r="B770" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="771" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A771" s="2">
+        <v>15995139</v>
+      </c>
+      <c r="B771" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="772" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A772" s="2">
+        <v>15995140</v>
+      </c>
+      <c r="B772" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="773" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A773" s="2">
+        <v>15995142</v>
+      </c>
+      <c r="B773" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="774" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A774" s="2">
+        <v>15995145</v>
+      </c>
+      <c r="B774" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="775" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A775" s="2">
+        <v>15995147</v>
+      </c>
+      <c r="B775" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="776" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A776" s="2">
+        <v>15995152</v>
+      </c>
+      <c r="B776" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="777" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A777" s="2">
+        <v>15995155</v>
+      </c>
+      <c r="B777" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="778" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A778" s="2">
+        <v>16006404</v>
+      </c>
+      <c r="B778" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="779" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A779" s="2">
+        <v>16006405</v>
+      </c>
+      <c r="B779" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="780" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A780" s="2">
+        <v>16006406</v>
+      </c>
+      <c r="B780" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="781" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A781" s="2">
+        <v>16006407</v>
+      </c>
+      <c r="B781" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="782" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A782" s="2">
+        <v>16006408</v>
+      </c>
+      <c r="B782" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="783" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A783" s="2">
+        <v>16006409</v>
+      </c>
+      <c r="B783" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="784" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A784" s="2">
+        <v>16006410</v>
+      </c>
+      <c r="B784" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="785" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A785" s="2">
+        <v>16006480</v>
+      </c>
+      <c r="B785" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="786" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A786" s="2">
+        <v>16006484</v>
+      </c>
+      <c r="B786" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="787" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A787" s="2">
+        <v>16006485</v>
+      </c>
+      <c r="B787" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="788" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A788" s="2">
+        <v>16006486</v>
+      </c>
+      <c r="B788" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="789" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A789" s="2">
+        <v>16006488</v>
+      </c>
+      <c r="B789" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="790" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A790" s="2">
+        <v>16006491</v>
+      </c>
+      <c r="B790" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="791" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A791" s="2">
+        <v>16006496</v>
+      </c>
+      <c r="B791" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="792" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A792" s="2">
+        <v>16006497</v>
+      </c>
+      <c r="B792" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="793" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A793" s="2">
+        <v>16006498</v>
+      </c>
+      <c r="B793" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="794" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A794" s="2">
+        <v>16027439</v>
+      </c>
+      <c r="B794" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="795" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A795" s="2">
+        <v>16027447</v>
+      </c>
+      <c r="B795" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="796" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A796" s="2">
+        <v>16027452</v>
+      </c>
+      <c r="B796" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="797" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A797" s="2">
+        <v>16027457</v>
+      </c>
+      <c r="B797" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="798" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A798" s="2">
+        <v>16027462</v>
+      </c>
+      <c r="B798" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="799" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A799" s="2">
+        <v>16027468</v>
+      </c>
+      <c r="B799" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="800" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A800" s="2">
+        <v>16027475</v>
+      </c>
+      <c r="B800" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="801" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A801" s="2">
+        <v>16027482</v>
+      </c>
+      <c r="B801" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="802" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A802" s="2">
+        <v>16027485</v>
+      </c>
+      <c r="B802" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="803" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A803" s="2">
+        <v>16027521</v>
+      </c>
+      <c r="B803" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="804" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A804" s="2">
+        <v>16027528</v>
+      </c>
+      <c r="B804" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="805" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A805" s="2">
+        <v>16027534</v>
+      </c>
+      <c r="B805" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="806" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A806" s="2">
+        <v>16027551</v>
+      </c>
+      <c r="B806" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="807" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A807" s="2">
+        <v>16027565</v>
+      </c>
+      <c r="B807" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="808" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A808" s="2">
+        <v>16027571</v>
+      </c>
+      <c r="B808" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="809" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A809" s="2">
+        <v>16027573</v>
+      </c>
+      <c r="B809" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="810" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A810" s="2">
+        <v>16027574</v>
+      </c>
+      <c r="B810" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="811" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A811" s="2">
+        <v>16027578</v>
+      </c>
+      <c r="B811" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="812" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A812" s="2">
+        <v>16027593</v>
+      </c>
+      <c r="B812" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="813" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A813" s="2">
+        <v>16027597</v>
+      </c>
+      <c r="B813" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="814" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A814" s="2">
+        <v>16027599</v>
+      </c>
+      <c r="B814" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="815" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A815" s="2">
+        <v>16027611</v>
+      </c>
+      <c r="B815" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="816" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A816" s="2">
+        <v>16051149</v>
+      </c>
+      <c r="B816" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="817" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A817" s="2">
+        <v>16051153</v>
+      </c>
+      <c r="B817" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="818" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A818" s="2">
+        <v>16051155</v>
+      </c>
+      <c r="B818" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="819" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A819" s="2">
+        <v>16051162</v>
+      </c>
+      <c r="B819" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="820" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A820" s="2">
+        <v>16051165</v>
+      </c>
+      <c r="B820" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="821" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A821" s="2">
+        <v>16051167</v>
+      </c>
+      <c r="B821" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="822" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A822" s="2">
+        <v>16051169</v>
+      </c>
+      <c r="B822" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="823" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A823" s="2">
+        <v>16051171</v>
+      </c>
+      <c r="B823" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="824" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A824" s="2">
+        <v>16051173</v>
+      </c>
+      <c r="B824" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="825" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A825" s="2">
+        <v>16051212</v>
+      </c>
+      <c r="B825" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="826" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A826" s="2">
+        <v>16051215</v>
+      </c>
+      <c r="B826" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="827" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A827" s="2">
+        <v>16051219</v>
+      </c>
+      <c r="B827" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="828" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A828" s="2">
+        <v>16051224</v>
+      </c>
+      <c r="B828" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="829" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A829" s="2">
+        <v>16051226</v>
+      </c>
+      <c r="B829" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="830" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A830" s="2">
+        <v>16051228</v>
+      </c>
+      <c r="B830" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="831" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A831" s="2">
+        <v>16051234</v>
+      </c>
+      <c r="B831" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="832" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A832" s="2">
+        <v>16053467</v>
+      </c>
+      <c r="B832" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="833" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A833" s="2">
+        <v>16053530</v>
+      </c>
+      <c r="B833" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="834" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A834" s="2">
+        <v>16053539</v>
+      </c>
+      <c r="B834" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="835" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A835" s="2">
+        <v>16053694</v>
+      </c>
+      <c r="B835" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="836" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A836" s="2">
+        <v>16053695</v>
+      </c>
+      <c r="B836" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="837" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A837" s="2">
+        <v>16053697</v>
+      </c>
+      <c r="B837" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="838" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A838" s="2">
+        <v>16053707</v>
+      </c>
+      <c r="B838" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="839" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A839" s="2">
+        <v>16053710</v>
+      </c>
+      <c r="B839" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="840" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A840" s="2">
+        <v>16053711</v>
+      </c>
+      <c r="B840" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="841" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A841" s="2">
+        <v>16053713</v>
+      </c>
+      <c r="B841" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="842" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A842" s="2">
+        <v>16053716</v>
+      </c>
+      <c r="B842" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="843" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A843" s="2">
+        <v>16053720</v>
+      </c>
+      <c r="B843" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="844" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A844" s="2">
+        <v>16053723</v>
+      </c>
+      <c r="B844" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="845" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A845" s="2">
+        <v>16053725</v>
+      </c>
+      <c r="B845" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="846" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A846" s="2">
+        <v>16053729</v>
+      </c>
+      <c r="B846" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="847" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A847" s="2">
+        <v>16053749</v>
+      </c>
+      <c r="B847" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="848" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A848" s="2">
+        <v>16069275</v>
+      </c>
+      <c r="B848" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="849" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A849" s="2">
+        <v>16069276</v>
+      </c>
+      <c r="B849" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="850" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A850" s="2">
+        <v>16069282</v>
+      </c>
+      <c r="B850" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="851" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A851" s="2">
+        <v>16069283</v>
+      </c>
+      <c r="B851" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="852" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A852" s="2">
+        <v>15972729</v>
+      </c>
+      <c r="B852" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="853" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A853" s="2">
+        <v>15972732</v>
+      </c>
+      <c r="B853" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="854" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A854" s="2">
+        <v>15972739</v>
+      </c>
+      <c r="B854" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="855" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A855" s="2">
+        <v>15972742</v>
+      </c>
+      <c r="B855" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="856" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A856" s="2">
+        <v>15972757</v>
+      </c>
+      <c r="B856" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="857" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A857" s="2">
+        <v>15972774</v>
+      </c>
+      <c r="B857" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="858" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A858" s="2">
+        <v>15972770</v>
+      </c>
+      <c r="B858" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="859" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A859" s="2">
+        <v>15972781</v>
+      </c>
+      <c r="B859" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="860" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A860" s="2">
+        <v>15972787</v>
+      </c>
+      <c r="B860" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="861" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A861" s="2">
+        <v>15972792</v>
+      </c>
+      <c r="B861" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="862" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A862" s="2">
+        <v>15972799</v>
+      </c>
+      <c r="B862" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="863" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A863" s="2">
+        <v>15972801</v>
+      </c>
+      <c r="B863" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="864" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A864" s="2">
+        <v>15972869</v>
+      </c>
+      <c r="B864" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="865" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A865" s="2">
+        <v>15972871</v>
+      </c>
+      <c r="B865" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="866" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A866" s="2">
+        <v>15972873</v>
+      </c>
+      <c r="B866" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="867" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A867" s="2">
+        <v>15972911</v>
+      </c>
+      <c r="B867" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="868" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A868" s="2">
+        <v>15972914</v>
+      </c>
+      <c r="B868" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="869" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A869" s="2">
+        <v>15972916</v>
+      </c>
+      <c r="B869" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="870" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A870" s="2">
+        <v>15972961</v>
+      </c>
+      <c r="B870" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="871" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A871" s="2">
+        <v>15972964</v>
+      </c>
+      <c r="B871" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="872" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A872" s="2">
+        <v>15973107</v>
+      </c>
+      <c r="B872" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="873" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A873" s="2">
+        <v>15973108</v>
+      </c>
+      <c r="B873" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="874" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A874" s="2">
+        <v>15973111</v>
+      </c>
+      <c r="B874" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="875" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A875" s="2">
+        <v>15973114</v>
+      </c>
+      <c r="B875" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="876" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A876" s="2">
+        <v>15973119</v>
+      </c>
+      <c r="B876" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="877" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A877" s="2">
+        <v>15973121</v>
+      </c>
+      <c r="B877" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="878" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A878" s="2">
+        <v>15973123</v>
+      </c>
+      <c r="B878" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="879" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A879" s="2">
+        <v>15973128</v>
+      </c>
+      <c r="B879" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="880" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A880" s="2">
+        <v>15973130</v>
+      </c>
+      <c r="B880" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="881" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A881" s="2">
+        <v>15973133</v>
+      </c>
+      <c r="B881" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="882" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A882" s="2">
+        <v>15973136</v>
+      </c>
+      <c r="B882" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="883" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A883" s="2">
+        <v>15973138</v>
+      </c>
+      <c r="B883" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="884" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A884" s="2">
+        <v>15973141</v>
+      </c>
+      <c r="B884" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="885" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A885" s="2">
+        <v>15973142</v>
+      </c>
+      <c r="B885" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="886" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A886" s="2">
+        <v>15973145</v>
+      </c>
+      <c r="B886" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="887" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A887" s="2">
+        <v>15973148</v>
+      </c>
+      <c r="B887" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="888" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A888" s="2">
+        <v>15974973</v>
+      </c>
+      <c r="B888" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="889" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A889" s="2">
+        <v>15975008</v>
+      </c>
+      <c r="B889" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A890" s="2">
+        <v>15975025</v>
+      </c>
+      <c r="B890" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="891" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A891" s="2">
+        <v>15975038</v>
+      </c>
+      <c r="B891" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A892" s="2">
+        <v>15975060</v>
+      </c>
+      <c r="B892" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A893" s="2">
+        <v>15975072</v>
+      </c>
+      <c r="B893" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="894" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A894" s="2">
+        <v>15975080</v>
+      </c>
+      <c r="B894" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A895" s="2">
+        <v>15975088</v>
+      </c>
+      <c r="B895" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="896" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A896" s="2">
+        <v>15975101</v>
+      </c>
+      <c r="B896" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="897" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A897" s="2">
+        <v>15975105</v>
+      </c>
+      <c r="B897" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A898" s="2">
+        <v>15975117</v>
+      </c>
+      <c r="B898" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="899" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A899" s="2">
+        <v>15975123</v>
+      </c>
+      <c r="B899" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A900" s="2">
+        <v>15975126</v>
+      </c>
+      <c r="B900" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="901" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A901" s="2">
+        <v>15975129</v>
+      </c>
+      <c r="B901" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="902" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A902" s="2">
+        <v>15975133</v>
+      </c>
+      <c r="B902" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="903" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A903" s="2">
+        <v>15975136</v>
+      </c>
+      <c r="B903" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="904" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A904" s="2">
+        <v>15975141</v>
+      </c>
+      <c r="B904" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="905" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A905" s="2">
+        <v>15975202</v>
+      </c>
+      <c r="B905" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="906" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A906" s="2">
+        <v>15975210</v>
+      </c>
+      <c r="B906" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="907" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A907" s="2">
+        <v>15975216</v>
+      </c>
+      <c r="B907" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="908" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A908" s="2">
+        <v>15975218</v>
+      </c>
+      <c r="B908" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A909" s="2">
+        <v>15975221</v>
+      </c>
+      <c r="B909" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="910" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A910" s="2">
+        <v>15975230</v>
+      </c>
+      <c r="B910" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="911" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A911" s="2">
+        <v>15975233</v>
+      </c>
+      <c r="B911" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="912" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A912" s="2">
+        <v>15975245</v>
+      </c>
+      <c r="B912" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="913" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A913" s="2">
+        <v>15975276</v>
+      </c>
+      <c r="B913" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="914" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A914" s="2">
+        <v>15975291</v>
+      </c>
+      <c r="B914" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="915" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A915" s="2">
+        <v>15975653</v>
+      </c>
+      <c r="B915" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="916" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A916" s="2">
+        <v>15975667</v>
+      </c>
+      <c r="B916" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="917" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A917" s="2">
+        <v>15975695</v>
+      </c>
+      <c r="B917" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="918" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A918" s="2">
+        <v>15975700</v>
+      </c>
+      <c r="B918" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="919" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A919" s="2">
+        <v>15975712</v>
+      </c>
+      <c r="B919" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="920" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A920" s="2">
+        <v>15975768</v>
+      </c>
+      <c r="B920" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="921" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A921" s="2">
+        <v>15979389</v>
+      </c>
+      <c r="B921" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="922" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A922" s="2">
+        <v>15979395</v>
+      </c>
+      <c r="B922" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="923" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A923" s="2">
+        <v>15979410</v>
+      </c>
+      <c r="B923" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="924" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A924" s="2">
+        <v>15979413</v>
+      </c>
+      <c r="B924" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="925" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A925" s="2">
+        <v>15979419</v>
+      </c>
+      <c r="B925" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="926" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A926" s="2">
+        <v>15979426</v>
+      </c>
+      <c r="B926" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="927" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A927" s="2">
+        <v>15979437</v>
+      </c>
+      <c r="B927" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="928" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A928" s="2">
+        <v>15979446</v>
+      </c>
+      <c r="B928" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="929" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A929" s="2">
+        <v>15979449</v>
+      </c>
+      <c r="B929" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="930" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A930" s="2">
+        <v>15979572</v>
+      </c>
+      <c r="B930" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="931" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A931" s="2">
+        <v>15979575</v>
+      </c>
+      <c r="B931" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="932" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A932" s="2">
+        <v>15979578</v>
+      </c>
+      <c r="B932" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="933" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A933" s="2">
+        <v>15979581</v>
+      </c>
+      <c r="B933" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="934" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A934" s="2">
+        <v>15979584</v>
+      </c>
+      <c r="B934" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="935" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A935" s="2">
+        <v>15979587</v>
+      </c>
+      <c r="B935" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="936" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A936" s="2">
+        <v>15979591</v>
+      </c>
+      <c r="B936" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="937" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A937" s="2">
+        <v>15979830</v>
+      </c>
+      <c r="B937" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="938" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A938" s="2">
+        <v>15979832</v>
+      </c>
+      <c r="B938" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="939" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A939" s="2">
+        <v>15979833</v>
+      </c>
+      <c r="B939" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="940" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A940" s="2">
+        <v>15979835</v>
+      </c>
+      <c r="B940" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="941" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A941" s="2">
+        <v>15979858</v>
+      </c>
+      <c r="B941" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="942" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A942" s="2">
+        <v>15979862</v>
+      </c>
+      <c r="B942" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="943" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A943" s="2">
+        <v>15979866</v>
+      </c>
+      <c r="B943" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="944" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A944" s="2">
+        <v>15979883</v>
+      </c>
+      <c r="B944" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="945" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A945" s="2">
+        <v>15979885</v>
+      </c>
+      <c r="B945" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="946" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A946" s="2">
+        <v>15979886</v>
+      </c>
+      <c r="B946" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="947" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A947" s="2">
+        <v>15979890</v>
+      </c>
+      <c r="B947" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="948" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A948" s="2">
+        <v>15979896</v>
+      </c>
+      <c r="B948" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="949" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A949" s="2">
+        <v>15979901</v>
+      </c>
+      <c r="B949" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="950" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A950" s="2">
+        <v>15979903</v>
+      </c>
+      <c r="B950" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="951" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A951" s="2">
+        <v>15979907</v>
+      </c>
+      <c r="B951" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="952" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A952" s="2">
+        <v>15979912</v>
+      </c>
+      <c r="B952" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="953" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A953" s="2">
+        <v>15979923</v>
+      </c>
+      <c r="B953" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="954" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A954" s="2">
+        <v>15979928</v>
+      </c>
+      <c r="B954" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="955" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A955" s="2">
+        <v>15979931</v>
+      </c>
+      <c r="B955" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="956" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A956" s="2">
+        <v>15980025</v>
+      </c>
+      <c r="B956" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="957" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A957" s="2">
+        <v>15980034</v>
+      </c>
+      <c r="B957" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="958" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A958" s="2">
+        <v>15980042</v>
+      </c>
+      <c r="B958" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="959" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A959" s="2">
+        <v>15980050</v>
+      </c>
+      <c r="B959" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="960" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A960" s="2">
+        <v>15980055</v>
+      </c>
+      <c r="B960" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="961" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A961" s="2">
+        <v>15980061</v>
+      </c>
+      <c r="B961" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="962" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A962" s="2">
+        <v>15980065</v>
+      </c>
+      <c r="B962" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="963" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A963" s="2">
+        <v>15980081</v>
+      </c>
+      <c r="B963" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="964" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A964" s="2">
+        <v>15980313</v>
+      </c>
+      <c r="B964" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="965" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A965" s="2">
+        <v>15980319</v>
+      </c>
+      <c r="B965" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="966" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A966" s="2">
+        <v>15980324</v>
+      </c>
+      <c r="B966" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="967" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A967" s="2">
+        <v>15980333</v>
+      </c>
+      <c r="B967" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="968" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A968" s="2">
+        <v>15980337</v>
+      </c>
+      <c r="B968" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="969" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A969" s="2">
+        <v>15980346</v>
+      </c>
+      <c r="B969" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="970" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A970" s="2">
+        <v>15980761</v>
+      </c>
+      <c r="B970" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="971" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A971" s="2">
+        <v>15980762</v>
+      </c>
+      <c r="B971" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="972" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A972" s="2">
+        <v>15980783</v>
+      </c>
+      <c r="B972" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="973" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A973" s="2">
+        <v>15980784</v>
+      </c>
+      <c r="B973" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="974" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A974" s="2">
+        <v>15980785</v>
+      </c>
+      <c r="B974" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="975" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A975" s="2">
+        <v>15980786</v>
+      </c>
+      <c r="B975" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="976" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A976" s="2">
+        <v>15980788</v>
+      </c>
+      <c r="B976" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="977" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A977" s="2">
+        <v>15980789</v>
+      </c>
+      <c r="B977" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="978" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A978" s="2">
+        <v>15980790</v>
+      </c>
+      <c r="B978" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="979" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A979" s="2">
+        <v>15980791</v>
+      </c>
+      <c r="B979" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="980" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A980" s="2">
+        <v>15980793</v>
+      </c>
+      <c r="B980" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="981" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A981" s="2">
+        <v>15980832</v>
+      </c>
+      <c r="B981" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="982" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A982" s="2">
+        <v>15980835</v>
+      </c>
+      <c r="B982" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="983" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A983" s="2">
+        <v>15980836</v>
+      </c>
+      <c r="B983" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="984" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A984" s="2">
+        <v>15980838</v>
+      </c>
+      <c r="B984" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="985" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A985" s="2">
+        <v>15980841</v>
+      </c>
+      <c r="B985" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="986" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A986" s="2">
+        <v>15980843</v>
+      </c>
+      <c r="B986" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="987" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A987" s="2">
+        <v>15980844</v>
+      </c>
+      <c r="B987" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="988" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A988" s="2">
+        <v>15980847</v>
+      </c>
+      <c r="B988" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="989" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A989" s="2">
+        <v>15980848</v>
+      </c>
+      <c r="B989" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="990" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A990" s="2">
+        <v>15980850</v>
+      </c>
+      <c r="B990" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="991" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A991" s="2">
+        <v>15980851</v>
+      </c>
+      <c r="B991" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="992" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A992" s="2">
+        <v>15980854</v>
+      </c>
+      <c r="B992" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="993" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A993" s="2">
+        <v>16479220</v>
+      </c>
+      <c r="B993" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="994" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A994" s="2">
+        <v>16487346</v>
+      </c>
+      <c r="B994" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="995" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A995" s="2">
+        <v>16451475</v>
+      </c>
+      <c r="B995" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="996" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A996" s="2">
+        <v>16489418</v>
+      </c>
+      <c r="B996" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="997" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A997" s="2">
+        <v>16490374</v>
+      </c>
+      <c r="B997" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="998" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A998" s="2">
+        <v>16490377</v>
+      </c>
+      <c r="B998" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="999" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A999" s="2">
+        <v>16490415</v>
+      </c>
+      <c r="B999" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1000" s="2">
+        <v>16490416</v>
+      </c>
+      <c r="B1000" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1001" s="2">
+        <v>16490417</v>
+      </c>
+      <c r="B1001" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1002" s="2">
+        <v>16490419</v>
+      </c>
+      <c r="B1002" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1003" s="2">
+        <v>16490421</v>
+      </c>
+      <c r="B1003" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1004" s="2">
+        <v>16490423</v>
+      </c>
+      <c r="B1004" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1005" s="2">
+        <v>16490425</v>
+      </c>
+      <c r="B1005" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1006" s="2">
+        <v>16490426</v>
+      </c>
+      <c r="B1006" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1007" s="2">
+        <v>16490427</v>
+      </c>
+      <c r="B1007" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1008" s="2">
+        <v>16490428</v>
+      </c>
+      <c r="B1008" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1009" s="2">
+        <v>16490429</v>
+      </c>
+      <c r="B1009" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1010" s="2">
+        <v>16490431</v>
+      </c>
+      <c r="B1010" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1011" s="2">
+        <v>16490433</v>
+      </c>
+      <c r="B1011" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1012" s="2">
+        <v>16490434</v>
+      </c>
+      <c r="B1012" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1013" s="2">
+        <v>16490435</v>
+      </c>
+      <c r="B1013" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1014" s="2">
+        <v>16490437</v>
+      </c>
+      <c r="B1014" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1015" s="2">
+        <v>16490438</v>
+      </c>
+      <c r="B1015" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1016" s="2">
+        <v>16490439</v>
+      </c>
+      <c r="B1016" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1017" s="2">
+        <v>16490441</v>
+      </c>
+      <c r="B1017" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1018" s="2">
+        <v>16490442</v>
+      </c>
+      <c r="B1018" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1019" s="2">
+        <v>16490443</v>
+      </c>
+      <c r="B1019" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1020" s="2">
+        <v>16490444</v>
+      </c>
+      <c r="B1020" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1021" s="2">
+        <v>16490445</v>
+      </c>
+      <c r="B1021" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1022" s="2">
+        <v>16490446</v>
+      </c>
+      <c r="B1022" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1023" s="2">
+        <v>16490447</v>
+      </c>
+      <c r="B1023" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1024" s="2">
+        <v>16490448</v>
+      </c>
+      <c r="B1024" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1025" s="2">
+        <v>16490450</v>
+      </c>
+      <c r="B1025" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1026" s="2">
+        <v>16490452</v>
+      </c>
+      <c r="B1026" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1027" s="2">
+        <v>16490453</v>
+      </c>
+      <c r="B1027" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1028" s="2">
+        <v>16490454</v>
+      </c>
+      <c r="B1028" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1029" s="2">
+        <v>16490455</v>
+      </c>
+      <c r="B1029" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1030" s="2">
+        <v>16490475</v>
+      </c>
+      <c r="B1030" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1031" s="2">
+        <v>16490476</v>
+      </c>
+      <c r="B1031" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1032" s="2">
+        <v>16490477</v>
+      </c>
+      <c r="B1032" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1033" s="2">
+        <v>16490479</v>
+      </c>
+      <c r="B1033" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1034" s="2">
+        <v>16490481</v>
+      </c>
+      <c r="B1034" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1035" s="2">
+        <v>16490482</v>
+      </c>
+      <c r="B1035" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1036" s="2">
+        <v>16490483</v>
+      </c>
+      <c r="B1036" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1037" s="2">
+        <v>16490484</v>
+      </c>
+      <c r="B1037" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1038" s="2">
+        <v>16490485</v>
+      </c>
+      <c r="B1038" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1039" s="2">
+        <v>16490486</v>
+      </c>
+      <c r="B1039" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1040" s="2">
+        <v>16490487</v>
+      </c>
+      <c r="B1040" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1041" s="2">
+        <v>16490488</v>
+      </c>
+      <c r="B1041" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1042" s="2">
+        <v>16490490</v>
+      </c>
+      <c r="B1042" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1043" s="2">
+        <v>16490491</v>
+      </c>
+      <c r="B1043" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1044" s="2">
+        <v>16490492</v>
+      </c>
+      <c r="B1044" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1045" s="2">
+        <v>16490493</v>
+      </c>
+      <c r="B1045" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1046" s="2">
+        <v>16490494</v>
+      </c>
+      <c r="B1046" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1047" s="2">
+        <v>16490495</v>
+      </c>
+      <c r="B1047" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1048" s="2">
+        <v>16490496</v>
+      </c>
+      <c r="B1048" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1049" s="2">
+        <v>16490497</v>
+      </c>
+      <c r="B1049" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1050" s="2">
+        <v>16490498</v>
+      </c>
+      <c r="B1050" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1051" s="2">
+        <v>16490499</v>
+      </c>
+      <c r="B1051" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1052" s="2">
+        <v>16490500</v>
+      </c>
+      <c r="B1052" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1053" s="2">
+        <v>16490501</v>
+      </c>
+      <c r="B1053" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1054" s="2">
+        <v>16490502</v>
+      </c>
+      <c r="B1054" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1055" s="2">
+        <v>16490503</v>
+      </c>
+      <c r="B1055" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1056" s="2">
+        <v>16490504</v>
+      </c>
+      <c r="B1056" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1057" s="2">
+        <v>16490505</v>
+      </c>
+      <c r="B1057" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1058" s="2">
+        <v>16490506</v>
+      </c>
+      <c r="B1058" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1059" s="2">
+        <v>16490508</v>
+      </c>
+      <c r="B1059" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1060" s="2">
+        <v>16490509</v>
+      </c>
+      <c r="B1060" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1061" s="2">
+        <v>16490510</v>
+      </c>
+      <c r="B1061" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1062" s="2">
+        <v>16490511</v>
+      </c>
+      <c r="B1062" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1063" s="2">
+        <v>16490512</v>
+      </c>
+      <c r="B1063" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1064" s="2">
+        <v>16490513</v>
+      </c>
+      <c r="B1064" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1065" s="2">
+        <v>16490514</v>
+      </c>
+      <c r="B1065" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1066" s="5">
+        <v>16490521</v>
+      </c>
+      <c r="B1066" s="5" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1067" s="5">
+        <v>16490522</v>
+      </c>
+      <c r="B1067" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1068" s="4">
+        <v>16490523</v>
+      </c>
+      <c r="B1068" s="4" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1069" s="4">
+        <v>16490524</v>
+      </c>
+      <c r="B1069" s="4" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1070" s="4">
+        <v>16490525</v>
+      </c>
+      <c r="B1070" s="4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1071" s="4">
+        <v>16490526</v>
+      </c>
+      <c r="B1071" s="4" t="s">
+        <v>437</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
:technologist: New instances & modified codes
</commit_message>
<xml_diff>
--- a/python-helpers/all-done.xlsx
+++ b/python-helpers/all-done.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\repos\bin-packing\python-helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAF7831-1649-447F-B0A8-0A7F2F25DA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E74182D-4CCD-4C6D-A43E-50DDEAE9F0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="603">
   <si>
     <t>Job number</t>
   </si>
@@ -1350,6 +1351,501 @@
   </si>
   <si>
     <t>SdLlIcry</t>
+  </si>
+  <si>
+    <t>zdLkaQvm</t>
+  </si>
+  <si>
+    <t>uieWjOkR</t>
+  </si>
+  <si>
+    <t>diUOPvuA</t>
+  </si>
+  <si>
+    <t>GodtJFWU</t>
+  </si>
+  <si>
+    <t>OqTwmsQb</t>
+  </si>
+  <si>
+    <t>naocvWsL</t>
+  </si>
+  <si>
+    <t>htxczmDp</t>
+  </si>
+  <si>
+    <t>FNXgiSLd</t>
+  </si>
+  <si>
+    <t>GyLUlRuv</t>
+  </si>
+  <si>
+    <t>SHFkUIXh</t>
+  </si>
+  <si>
+    <t>DqWHcBsn</t>
+  </si>
+  <si>
+    <t>nqAuRYyU</t>
+  </si>
+  <si>
+    <t>MXydAJCL</t>
+  </si>
+  <si>
+    <t>oWErdxyG</t>
+  </si>
+  <si>
+    <t>IPpRXeTE</t>
+  </si>
+  <si>
+    <t>rlCSwNkA</t>
+  </si>
+  <si>
+    <t>nVERgPdO</t>
+  </si>
+  <si>
+    <t>yujEvOIT</t>
+  </si>
+  <si>
+    <t>oBnqUYVs</t>
+  </si>
+  <si>
+    <t>sbwnhoAE</t>
+  </si>
+  <si>
+    <t>imUFwSvR</t>
+  </si>
+  <si>
+    <t>JxcUQjfF</t>
+  </si>
+  <si>
+    <t>wEbyFDPV</t>
+  </si>
+  <si>
+    <t>JxPdICwN</t>
+  </si>
+  <si>
+    <t>NREqJQzn</t>
+  </si>
+  <si>
+    <t>uqglDPbR</t>
+  </si>
+  <si>
+    <t>JqjPCUke</t>
+  </si>
+  <si>
+    <t>dKgYIWUD</t>
+  </si>
+  <si>
+    <t>NDQWwuOg</t>
+  </si>
+  <si>
+    <t>fLuKACsx</t>
+  </si>
+  <si>
+    <t>rRWmbyKu</t>
+  </si>
+  <si>
+    <t>OnHhDbNZ</t>
+  </si>
+  <si>
+    <t>bLRpaUwg</t>
+  </si>
+  <si>
+    <t>BcEDPdqf</t>
+  </si>
+  <si>
+    <t>IfKCmRkQ</t>
+  </si>
+  <si>
+    <t>bmSLWKwj</t>
+  </si>
+  <si>
+    <t>lRJmWyLu</t>
+  </si>
+  <si>
+    <t>QLtUGzAl</t>
+  </si>
+  <si>
+    <t>alHgCwyL</t>
+  </si>
+  <si>
+    <t>fHhOFDmA</t>
+  </si>
+  <si>
+    <t>kNSYOsGr</t>
+  </si>
+  <si>
+    <t>WGATFeDN</t>
+  </si>
+  <si>
+    <t>VweMofJt</t>
+  </si>
+  <si>
+    <t>zlNoikaG</t>
+  </si>
+  <si>
+    <t>YGvgDBkM</t>
+  </si>
+  <si>
+    <t>pyEisMlv</t>
+  </si>
+  <si>
+    <t>drMtibDZ</t>
+  </si>
+  <si>
+    <t>hPTuQyGI</t>
+  </si>
+  <si>
+    <t>ymiLCfPI</t>
+  </si>
+  <si>
+    <t>SGmfovks</t>
+  </si>
+  <si>
+    <t>XlPkZCai</t>
+  </si>
+  <si>
+    <t>VXwcuHtC</t>
+  </si>
+  <si>
+    <t>hActDNQo</t>
+  </si>
+  <si>
+    <t>axvzTAXC</t>
+  </si>
+  <si>
+    <t>CyuieUft</t>
+  </si>
+  <si>
+    <t>gjeozHTF</t>
+  </si>
+  <si>
+    <t>tUsQiSqE</t>
+  </si>
+  <si>
+    <t>fjZlBDCE</t>
+  </si>
+  <si>
+    <t>uvOebxmE</t>
+  </si>
+  <si>
+    <t>TCdFwkDt</t>
+  </si>
+  <si>
+    <t>fxRKDNcH</t>
+  </si>
+  <si>
+    <t>iFvUXBRg</t>
+  </si>
+  <si>
+    <t>AZltRIWy</t>
+  </si>
+  <si>
+    <t>DFmSEWyd</t>
+  </si>
+  <si>
+    <t>fUbejDqk</t>
+  </si>
+  <si>
+    <t>UvFNyQbg</t>
+  </si>
+  <si>
+    <t>aEjHTBNn</t>
+  </si>
+  <si>
+    <t>djrYueFz</t>
+  </si>
+  <si>
+    <t>wDRTqemi</t>
+  </si>
+  <si>
+    <t>WOLebuZi</t>
+  </si>
+  <si>
+    <t>ArWCDSft</t>
+  </si>
+  <si>
+    <t>mbrUGXak</t>
+  </si>
+  <si>
+    <t>hCyPLIzS</t>
+  </si>
+  <si>
+    <t>PYJRnqsV</t>
+  </si>
+  <si>
+    <t>VOGNAxpX</t>
+  </si>
+  <si>
+    <t>ZMYarctQ</t>
+  </si>
+  <si>
+    <t>iCSfMLXx</t>
+  </si>
+  <si>
+    <t>NkyzTsFm</t>
+  </si>
+  <si>
+    <t>jUiFwTeB</t>
+  </si>
+  <si>
+    <t>MCJtvAXx</t>
+  </si>
+  <si>
+    <t>iWxfpLmt</t>
+  </si>
+  <si>
+    <t>XbiMCABq</t>
+  </si>
+  <si>
+    <t>MIEdjoht</t>
+  </si>
+  <si>
+    <t>jbIJehLA</t>
+  </si>
+  <si>
+    <t>JUPtHeqj</t>
+  </si>
+  <si>
+    <t>SDdHszOJ</t>
+  </si>
+  <si>
+    <t>GaEILpfq</t>
+  </si>
+  <si>
+    <t>fvxTNIBW</t>
+  </si>
+  <si>
+    <t>RPBkTgMV</t>
+  </si>
+  <si>
+    <t>JxNOsliA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JxNOsliA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> juBgYVvf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vakxRBUA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OrjDCZbJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GMgVTpxq</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GHWLmhZS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RPBkTgMV</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GaEILpfq</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BHqKQXmn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rHSUYKGs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vLNXRVpz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jvxptGTk</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PhtjrwJf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GSEmqMyl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XigxluIK</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wZHdCkpX</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lntqNuED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tzjYGpwI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pHQsRZKk</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> oIRFzMWH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cFVvZhgX</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ErDhgawM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pDCZBLSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eoxHlfiG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fWtuGQMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sONKeBzd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> uFRWpdoO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> iLnOPUcs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YtemhiJy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sLZlbyFe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SwYzeoDW</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TJzvZmld</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HlAPdMpB</t>
+  </si>
+  <si>
+    <t>RAojCOHs</t>
+  </si>
+  <si>
+    <t>YKdhJxAi</t>
+  </si>
+  <si>
+    <t>riWglYAK</t>
+  </si>
+  <si>
+    <t>mVXOhGys</t>
+  </si>
+  <si>
+    <t>aDqkfnpg</t>
+  </si>
+  <si>
+    <t>XoDnmWeF</t>
+  </si>
+  <si>
+    <t>KYeNVyfh</t>
+  </si>
+  <si>
+    <t>vUTlOQsA</t>
+  </si>
+  <si>
+    <t>RzNWCjXP</t>
+  </si>
+  <si>
+    <t>FTogPXwZ</t>
+  </si>
+  <si>
+    <t>NDbwxLPr</t>
+  </si>
+  <si>
+    <t>eYZySiRd</t>
+  </si>
+  <si>
+    <t>WjnhZMfa</t>
+  </si>
+  <si>
+    <t>FyJPIvgd</t>
+  </si>
+  <si>
+    <t>FZjIMKrV</t>
+  </si>
+  <si>
+    <t>oQgROGMw</t>
+  </si>
+  <si>
+    <t>FxdeQawv</t>
+  </si>
+  <si>
+    <t>FNlDhBXc</t>
+  </si>
+  <si>
+    <t>hWQMlVBX</t>
+  </si>
+  <si>
+    <t>RpCNUqQf</t>
+  </si>
+  <si>
+    <t>cXdsWbvY</t>
+  </si>
+  <si>
+    <t>vylKYrWh</t>
+  </si>
+  <si>
+    <t>aPjqIogf</t>
+  </si>
+  <si>
+    <t>hzlmDZoH</t>
+  </si>
+  <si>
+    <t>DSjNhrmA</t>
+  </si>
+  <si>
+    <t>DsFoSfbg</t>
+  </si>
+  <si>
+    <t>xEKhYJCW</t>
+  </si>
+  <si>
+    <t>nKcAMZSy</t>
+  </si>
+  <si>
+    <t>NdlxrTHo</t>
+  </si>
+  <si>
+    <t>ObYfiIvW</t>
+  </si>
+  <si>
+    <t>nQjoRCMq</t>
+  </si>
+  <si>
+    <t>FVgsdLiS</t>
+  </si>
+  <si>
+    <t>fBeAoHcv</t>
+  </si>
+  <si>
+    <t>ZwyDRWFm</t>
+  </si>
+  <si>
+    <t>MdLacIwQ</t>
+  </si>
+  <si>
+    <t>SIOfKsxe</t>
+  </si>
+  <si>
+    <t>zOfaqIRs</t>
+  </si>
+  <si>
+    <t>pUiWJxVG</t>
+  </si>
+  <si>
+    <t>UFsolZCO</t>
+  </si>
+  <si>
+    <t>gGfzYbcM</t>
+  </si>
+  <si>
+    <t>wkIDacKh</t>
+  </si>
+  <si>
+    <t>KPznNAgR</t>
   </si>
 </sst>
 </file>
@@ -1412,7 +1908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1425,6 +1921,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1707,10 +2206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1071"/>
+  <dimension ref="A1:C1236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1052" workbookViewId="0">
-      <selection activeCell="A1066" sqref="A1066:B1071"/>
+    <sheetView tabSelected="1" topLeftCell="A1129" workbookViewId="0">
+      <selection activeCell="A1195" sqref="A1195:B1236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10288,7 +10787,1341 @@
         <v>437</v>
       </c>
     </row>
+    <row r="1072" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1072" s="1">
+        <v>16491210</v>
+      </c>
+      <c r="B1072" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1073" s="2">
+        <v>16491244</v>
+      </c>
+      <c r="B1073" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1074" s="2">
+        <v>16491246</v>
+      </c>
+      <c r="B1074" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1075" s="2">
+        <v>16491247</v>
+      </c>
+      <c r="B1075" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1076" s="2">
+        <v>16491248</v>
+      </c>
+      <c r="B1076" s="2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1077" s="2">
+        <v>16491263</v>
+      </c>
+      <c r="B1077" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1078" s="2">
+        <v>16491273</v>
+      </c>
+      <c r="B1078" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1079" s="2">
+        <v>16491274</v>
+      </c>
+      <c r="B1079" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1080" s="2">
+        <v>16491276</v>
+      </c>
+      <c r="B1080" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1081" s="2">
+        <v>16491277</v>
+      </c>
+      <c r="B1081" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1082" s="2">
+        <v>16491278</v>
+      </c>
+      <c r="B1082" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1083" s="2">
+        <v>16491285</v>
+      </c>
+      <c r="B1083" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1084" s="2">
+        <v>16491298</v>
+      </c>
+      <c r="B1084" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1085" s="2">
+        <v>16491299</v>
+      </c>
+      <c r="B1085" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1086" s="2">
+        <v>16491301</v>
+      </c>
+      <c r="B1086" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1087" s="2">
+        <v>16491302</v>
+      </c>
+      <c r="B1087" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1088" s="2">
+        <v>16491304</v>
+      </c>
+      <c r="B1088" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1089" s="2">
+        <v>16491305</v>
+      </c>
+      <c r="B1089" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1090" s="2">
+        <v>16491306</v>
+      </c>
+      <c r="B1090" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1091" s="2">
+        <v>16491308</v>
+      </c>
+      <c r="B1091" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1092" s="2">
+        <v>16491312</v>
+      </c>
+      <c r="B1092" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1093" s="2">
+        <v>16491319</v>
+      </c>
+      <c r="B1093" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1094" s="2">
+        <v>16491320</v>
+      </c>
+      <c r="B1094" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1095" s="2">
+        <v>16491322</v>
+      </c>
+      <c r="B1095" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1096" s="2">
+        <v>16491324</v>
+      </c>
+      <c r="B1096" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1097" s="2">
+        <v>16491326</v>
+      </c>
+      <c r="B1097" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1098" s="2">
+        <v>16491330</v>
+      </c>
+      <c r="B1098" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1099" s="2">
+        <v>16491331</v>
+      </c>
+      <c r="B1099" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1100" s="2">
+        <v>16491333</v>
+      </c>
+      <c r="B1100" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1101" s="2">
+        <v>16491334</v>
+      </c>
+      <c r="B1101" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1102" s="2">
+        <v>16491335</v>
+      </c>
+      <c r="B1102" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1103" s="2">
+        <v>16491336</v>
+      </c>
+      <c r="B1103" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1104" s="2">
+        <v>16491337</v>
+      </c>
+      <c r="B1104" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1105" s="2">
+        <v>16491339</v>
+      </c>
+      <c r="B1105" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1106" s="2">
+        <v>16491353</v>
+      </c>
+      <c r="B1106" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1107" s="2">
+        <v>16491359</v>
+      </c>
+      <c r="B1107" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1108" s="2">
+        <v>16491366</v>
+      </c>
+      <c r="B1108" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1109" s="2">
+        <v>16491367</v>
+      </c>
+      <c r="B1109" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1110" s="2">
+        <v>16491369</v>
+      </c>
+      <c r="B1110" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1111" s="2">
+        <v>16491370</v>
+      </c>
+      <c r="B1111" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1112" s="2">
+        <v>16491371</v>
+      </c>
+      <c r="B1112" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1113" s="2">
+        <v>16491373</v>
+      </c>
+      <c r="B1113" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1114" s="2">
+        <v>16491375</v>
+      </c>
+      <c r="B1114" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1115" s="2">
+        <v>16491377</v>
+      </c>
+      <c r="B1115" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1116" s="2">
+        <v>16491378</v>
+      </c>
+      <c r="B1116" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1117" s="2">
+        <v>16491379</v>
+      </c>
+      <c r="B1117" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1118" s="2">
+        <v>16491380</v>
+      </c>
+      <c r="B1118" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1119" s="2">
+        <v>16491381</v>
+      </c>
+      <c r="B1119" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1120" s="2">
+        <v>16491389</v>
+      </c>
+      <c r="B1120" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1121" s="2">
+        <v>16491391</v>
+      </c>
+      <c r="B1121" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1122" s="2">
+        <v>16491400</v>
+      </c>
+      <c r="B1122" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1123" s="2">
+        <v>16491401</v>
+      </c>
+      <c r="B1123" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1124" s="2">
+        <v>16491402</v>
+      </c>
+      <c r="B1124" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1125" s="2">
+        <v>16491403</v>
+      </c>
+      <c r="B1125" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1126" s="2">
+        <v>16491406</v>
+      </c>
+      <c r="B1126" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1127" s="2">
+        <v>16491407</v>
+      </c>
+      <c r="B1127" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1128" s="2">
+        <v>16491408</v>
+      </c>
+      <c r="B1128" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1129" s="2">
+        <v>16491419</v>
+      </c>
+      <c r="B1129" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1130" s="2">
+        <v>16491421</v>
+      </c>
+      <c r="B1130" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1131" s="2">
+        <v>16491464</v>
+      </c>
+      <c r="B1131" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1132" s="2">
+        <v>16491474</v>
+      </c>
+      <c r="B1132" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1133" s="2">
+        <v>16491478</v>
+      </c>
+      <c r="B1133" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1134" s="2">
+        <v>16491483</v>
+      </c>
+      <c r="B1134" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1135" s="2">
+        <v>16491496</v>
+      </c>
+      <c r="B1135" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1136" s="2">
+        <v>16492757</v>
+      </c>
+      <c r="B1136" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1137" s="2">
+        <v>16492758</v>
+      </c>
+      <c r="B1137" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1138" s="2">
+        <v>16492759</v>
+      </c>
+      <c r="B1138" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1139" s="2">
+        <v>16492760</v>
+      </c>
+      <c r="B1139" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1140" s="2">
+        <v>16492761</v>
+      </c>
+      <c r="B1140" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1141" s="2">
+        <v>16492762</v>
+      </c>
+      <c r="B1141" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1142" s="2">
+        <v>16492765</v>
+      </c>
+      <c r="B1142" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1143" s="2">
+        <v>16492766</v>
+      </c>
+      <c r="B1143" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1144" s="2">
+        <v>16492767</v>
+      </c>
+      <c r="B1144" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1145" s="2">
+        <v>16492768</v>
+      </c>
+      <c r="B1145" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1146" s="2">
+        <v>16492770</v>
+      </c>
+      <c r="B1146" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1147" s="2">
+        <v>16492771</v>
+      </c>
+      <c r="B1147" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1148" s="2">
+        <v>16492774</v>
+      </c>
+      <c r="B1148" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1149" s="2">
+        <v>16496603</v>
+      </c>
+      <c r="B1149" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1150" s="2">
+        <v>16496604</v>
+      </c>
+      <c r="B1150" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1151" s="2">
+        <v>16496608</v>
+      </c>
+      <c r="B1151" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1152">
+        <v>16496743</v>
+      </c>
+      <c r="B1152" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1153" s="2">
+        <v>16496738</v>
+      </c>
+      <c r="B1153" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1154" s="2">
+        <v>16496732</v>
+      </c>
+      <c r="B1154" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1155">
+        <v>16496726</v>
+      </c>
+      <c r="B1155" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1156">
+        <v>16496722</v>
+      </c>
+      <c r="B1156" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1157">
+        <v>16496719</v>
+      </c>
+      <c r="B1157" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1158">
+        <v>16501231</v>
+      </c>
+      <c r="B1158" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1159">
+        <v>16501242</v>
+      </c>
+      <c r="B1159" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1160">
+        <v>16501230</v>
+      </c>
+      <c r="B1160" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1161">
+        <v>16501191</v>
+      </c>
+      <c r="B1161" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1162">
+        <v>16501191</v>
+      </c>
+      <c r="B1162" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1163">
+        <v>16501193</v>
+      </c>
+      <c r="B1163" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1164">
+        <v>16501195</v>
+      </c>
+      <c r="B1164" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1165">
+        <v>16501197</v>
+      </c>
+      <c r="B1165" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1166">
+        <v>16501227</v>
+      </c>
+      <c r="B1166" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1167">
+        <v>16501228</v>
+      </c>
+      <c r="B1167" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1168">
+        <v>16501230</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1169">
+        <v>16501231</v>
+      </c>
+      <c r="B1169" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1170">
+        <v>16501256</v>
+      </c>
+      <c r="B1170" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1171">
+        <v>16501259</v>
+      </c>
+      <c r="B1171" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1172">
+        <v>16501260</v>
+      </c>
+      <c r="B1172" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1173">
+        <v>16501271</v>
+      </c>
+      <c r="B1173" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1174">
+        <v>16501328</v>
+      </c>
+      <c r="B1174" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1175">
+        <v>16501330</v>
+      </c>
+      <c r="B1175" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1176">
+        <v>16501332</v>
+      </c>
+      <c r="B1176" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1177">
+        <v>16501333</v>
+      </c>
+      <c r="B1177" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1178">
+        <v>16501335</v>
+      </c>
+      <c r="B1178" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1179">
+        <v>16501336</v>
+      </c>
+      <c r="B1179" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1180">
+        <v>16501337</v>
+      </c>
+      <c r="B1180" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1181">
+        <v>16501338</v>
+      </c>
+      <c r="B1181" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1182">
+        <v>16501339</v>
+      </c>
+      <c r="B1182" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1183">
+        <v>16501341</v>
+      </c>
+      <c r="B1183" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1184">
+        <v>16501344</v>
+      </c>
+      <c r="B1184" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1185">
+        <v>16501346</v>
+      </c>
+      <c r="B1185" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1186">
+        <v>16501347</v>
+      </c>
+      <c r="B1186" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1187">
+        <v>16501349</v>
+      </c>
+      <c r="B1187" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1188">
+        <v>16501350</v>
+      </c>
+      <c r="B1188" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1189">
+        <v>16501351</v>
+      </c>
+      <c r="B1189" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1190">
+        <v>16501353</v>
+      </c>
+      <c r="B1190" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1191">
+        <v>16501357</v>
+      </c>
+      <c r="B1191" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1192">
+        <v>16501358</v>
+      </c>
+      <c r="B1192" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1193">
+        <v>16501359</v>
+      </c>
+      <c r="B1193" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1194">
+        <v>16501362</v>
+      </c>
+      <c r="B1194" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1195" s="6">
+        <v>16496622</v>
+      </c>
+      <c r="B1195" s="6" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1196" s="6">
+        <v>16496627</v>
+      </c>
+      <c r="B1196" s="6" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1197" s="6">
+        <v>16496628</v>
+      </c>
+      <c r="B1197" s="6" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1198" s="6">
+        <v>16496630</v>
+      </c>
+      <c r="B1198" s="6" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1199" s="6">
+        <v>16496634</v>
+      </c>
+      <c r="B1199" s="6" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1200" s="6">
+        <v>16496635</v>
+      </c>
+      <c r="B1200" s="6" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1201" s="6">
+        <v>16496636</v>
+      </c>
+      <c r="B1201" s="6" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1202" s="6">
+        <v>16496637</v>
+      </c>
+      <c r="B1202" s="6" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1203" s="6">
+        <v>16496640</v>
+      </c>
+      <c r="B1203" s="6" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1204" s="6">
+        <v>16496641</v>
+      </c>
+      <c r="B1204" s="6" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1205" s="6">
+        <v>16496642</v>
+      </c>
+      <c r="B1205" s="6" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1206" s="6">
+        <v>16496648</v>
+      </c>
+      <c r="B1206" s="6" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1207" s="6">
+        <v>16496666</v>
+      </c>
+      <c r="B1207" s="6" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1208" s="6">
+        <v>16496668</v>
+      </c>
+      <c r="B1208" s="6" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1209" s="6">
+        <v>16496670</v>
+      </c>
+      <c r="B1209" s="6" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1210" s="6">
+        <v>16496671</v>
+      </c>
+      <c r="B1210" s="6" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1211" s="6">
+        <v>16496672</v>
+      </c>
+      <c r="B1211" s="6" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1212" s="6">
+        <v>16496673</v>
+      </c>
+      <c r="B1212" s="6" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1213" s="6">
+        <v>16496674</v>
+      </c>
+      <c r="B1213" s="6" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1214" s="6">
+        <v>16496676</v>
+      </c>
+      <c r="B1214" s="6" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1215" s="6">
+        <v>16496678</v>
+      </c>
+      <c r="B1215" s="6" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1216" s="6">
+        <v>16496683</v>
+      </c>
+      <c r="B1216" s="6" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1217" s="6">
+        <v>16496685</v>
+      </c>
+      <c r="B1217" s="6" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1218" s="6">
+        <v>16496686</v>
+      </c>
+      <c r="B1218" s="6" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1219" s="6">
+        <v>16496687</v>
+      </c>
+      <c r="B1219" s="6" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1220" s="6">
+        <v>16496690</v>
+      </c>
+      <c r="B1220" s="6" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1221" s="6">
+        <v>16496694</v>
+      </c>
+      <c r="B1221" s="6" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1222" s="6">
+        <v>16496700</v>
+      </c>
+      <c r="B1222" s="6" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1223" s="6">
+        <v>16496709</v>
+      </c>
+      <c r="B1223" s="6" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1224" s="6">
+        <v>16496712</v>
+      </c>
+      <c r="B1224" s="6" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1225" s="6">
+        <v>16496714</v>
+      </c>
+      <c r="B1225" s="6" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1226" s="6">
+        <v>16496715</v>
+      </c>
+      <c r="B1226" s="6" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1227" s="6">
+        <v>16496716</v>
+      </c>
+      <c r="B1227" s="6" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1228" s="6">
+        <v>16496718</v>
+      </c>
+      <c r="B1228" s="6" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1229" s="6">
+        <v>16496721</v>
+      </c>
+      <c r="B1229" s="6" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1230" s="6">
+        <v>16496723</v>
+      </c>
+      <c r="B1230" s="6" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1231" s="6">
+        <v>16496727</v>
+      </c>
+      <c r="B1231" s="6" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1232" s="6">
+        <v>16496733</v>
+      </c>
+      <c r="B1232" s="6" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1233" s="6">
+        <v>16496737</v>
+      </c>
+      <c r="B1233" s="6" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1234" s="6">
+        <v>16496745</v>
+      </c>
+      <c r="B1234" s="6" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1235" s="6">
+        <v>16496748</v>
+      </c>
+      <c r="B1235" s="6" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:2" ht="15" x14ac:dyDescent="0.3">
+      <c r="A1236" s="6">
+        <v>16496750</v>
+      </c>
+      <c r="B1236" s="6" t="s">
+        <v>602</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{030BE086-49B0-4540-A0DD-C445CD53601B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>